<commit_message>
Run w export and fixed setting wd
</commit_message>
<xml_diff>
--- a/lit_data/output/lit_summ.xlsx
+++ b/lit_data/output/lit_summ.xlsx
@@ -12,54 +12,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">slurry.major</t>
   </si>
   <si>
-    <t xml:space="preserve">DM.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">totN.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM.sd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH.sd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN.sd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">totN.sd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM.n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH.n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN.n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">totN.n</t>
+    <t xml:space="preserve">variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value.mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value.sd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value.n</t>
   </si>
   <si>
     <t xml:space="preserve">cattle</t>
   </si>
   <si>
+    <t xml:space="preserve">DM</t>
+  </si>
+  <si>
     <t xml:space="preserve">cattle and pig</t>
   </si>
   <si>
     <t xml:space="preserve">pig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totN</t>
   </si>
 </sst>
 </file>
@@ -407,152 +395,209 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
         <v>4.4</v>
       </c>
-      <c r="C2" t="n">
-        <v>7.66</v>
-      </c>
       <c r="D2" t="n">
-        <v>2.1</v>
+        <v>1.54</v>
       </c>
       <c r="E2" t="n">
-        <v>3.35</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.54</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.953</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.613</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="J2" t="n">
-        <v>59</v>
-      </c>
-      <c r="K2" t="n">
-        <v>59</v>
-      </c>
-      <c r="L2" t="n">
-        <v>59</v>
-      </c>
-      <c r="M2" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="n">
         <v>4.55</v>
       </c>
-      <c r="C3" t="n">
-        <v>8.16</v>
-      </c>
       <c r="D3" t="n">
-        <v>4.03</v>
+        <v>1.74</v>
       </c>
       <c r="E3" t="n">
-        <v>5.42</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1.74</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.0597</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.378</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.568</v>
-      </c>
-      <c r="J3" t="n">
-        <v>4</v>
-      </c>
-      <c r="K3" t="n">
-        <v>4</v>
-      </c>
-      <c r="L3" t="n">
-        <v>4</v>
-      </c>
-      <c r="M3" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2.43</v>
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>8.2</v>
+        <v>2.39</v>
       </c>
       <c r="D4" t="n">
-        <v>3.54</v>
+        <v>1.06</v>
       </c>
       <c r="E4" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>7.66</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.953</v>
+      </c>
+      <c r="E5" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8.16</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0597</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>8.16</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.391</v>
+      </c>
+      <c r="E7" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.613</v>
+      </c>
+      <c r="E8" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.378</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.819</v>
+      </c>
+      <c r="E10" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="E11" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5.42</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.568</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="n">
         <v>5.01</v>
       </c>
-      <c r="F4" t="n">
-        <v>1.02</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.392</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="I4" t="n">
+      <c r="D13" t="n">
         <v>0.652</v>
       </c>
-      <c r="J4" t="n">
-        <v>24</v>
-      </c>
-      <c r="K4" t="n">
-        <v>24</v>
-      </c>
-      <c r="L4" t="n">
-        <v>24</v>
-      </c>
-      <c r="M4" t="n">
-        <v>24</v>
+      <c r="E13" t="n">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>